<commit_message>
remove commas from data
</commit_message>
<xml_diff>
--- a/Data/Keogh coho adults.xlsx
+++ b/Data/Keogh coho adults.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kyle\Documents\GitHub\Keogh\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kylel\OneDrive\Documents\GitHub\Keogh\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6CC9EB3B-DB15-4D62-890F-34DB8C0014CD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26E5CBD9-20DB-4E4C-8D4C-164AB486DF7E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" xr2:uid="{D3423027-8619-42DD-B274-791D62593B68}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8985" xr2:uid="{D3423027-8619-42DD-B274-791D62593B68}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -74,7 +74,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -392,20 +392,23 @@
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="9.140625" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1998</v>
       </c>
@@ -413,7 +416,7 @@
         <v>8501</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1999</v>
       </c>
@@ -421,7 +424,7 @@
         <v>2887</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2000</v>
       </c>
@@ -429,7 +432,7 @@
         <v>1206</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2001</v>
       </c>
@@ -437,7 +440,7 @@
         <v>2175</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2002</v>
       </c>
@@ -445,7 +448,7 @@
         <v>3307</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2003</v>
       </c>
@@ -453,7 +456,7 @@
         <v>1162</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2004</v>
       </c>
@@ -461,7 +464,7 @@
         <v>1156</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2005</v>
       </c>
@@ -469,7 +472,7 @@
         <v>3347</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2006</v>
       </c>
@@ -477,7 +480,7 @@
         <v>1840</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2007</v>
       </c>
@@ -485,15 +488,15 @@
         <v>2780</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2008</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="1">
         <v>926</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2009</v>
       </c>
@@ -501,7 +504,7 @@
         <v>3390</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2010</v>
       </c>
@@ -509,7 +512,7 @@
         <v>2106</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2011</v>
       </c>
@@ -517,7 +520,7 @@
         <v>2129</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2012</v>
       </c>
@@ -525,7 +528,7 @@
         <v>4832</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2013</v>
       </c>
@@ -533,7 +536,7 @@
         <v>5594</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2014</v>
       </c>
@@ -541,15 +544,15 @@
         <v>12187</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2015</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="1">
         <v>697</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2016</v>
       </c>

</xml_diff>